<commit_message>
Fixes tiny data issue with quantization size for helath outcomes (was zero, now 1)
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/QSfHO/Quantization Size for Health Outcomes.xlsx
+++ b/InputData/add-outputs/QSfHO/Quantization Size for Health Outcomes.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\add-outputs\QSfHO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\add-outputs\QSfHO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4BFE5A-59BE-4BAC-B3E6-430CDB115521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3134398-E81F-46A9-8446-A733961D3B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11415" yWindow="510" windowWidth="43200" windowHeight="17235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="QSfHO" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -136,10 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -161,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,9 +213,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,26 +248,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,26 +283,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -485,14 +463,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,97 +478,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -608,25 +586,27 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>